<commit_message>
pivot data to long format
</commit_message>
<xml_diff>
--- a/extdata/biochem_dictionary.xlsx
+++ b/extdata/biochem_dictionary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ogradye\Documents\Davis_Strait\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ogradye\Documents\Davis_Strait\R_Working\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6FE9A5-8B61-4EE5-8E0A-F89D0010FAFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BED7CEB-B6CF-4C97-9EEF-4F99B9855657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BCS" sheetId="1" r:id="rId1"/>
@@ -1187,14 +1187,14 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.5546875" customWidth="1"/>
-    <col min="3" max="3" width="56.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" customWidth="1"/>
+    <col min="3" max="3" width="56.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1218,7 +1218,7 @@
       </c>
       <c r="D2" s="6"/>
     </row>
-    <row r="3" spans="1:4" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
@@ -1230,7 +1230,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>7</v>
       </c>
@@ -1242,7 +1242,7 @@
       </c>
       <c r="D4" s="12"/>
     </row>
-    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>9</v>
       </c>
@@ -1254,7 +1254,7 @@
       </c>
       <c r="D5" s="13"/>
     </row>
-    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>11</v>
       </c>
@@ -1266,7 +1266,7 @@
       </c>
       <c r="D6" s="13"/>
     </row>
-    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>13</v>
       </c>
@@ -1276,7 +1276,7 @@
       </c>
       <c r="D7" s="9"/>
     </row>
-    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>15</v>
       </c>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="D8" s="9"/>
     </row>
-    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>17</v>
       </c>
@@ -1296,7 +1296,7 @@
       </c>
       <c r="D9" s="9"/>
     </row>
-    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>19</v>
       </c>
@@ -1306,7 +1306,7 @@
       </c>
       <c r="D10" s="16"/>
     </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>21</v>
       </c>
@@ -1316,7 +1316,7 @@
       </c>
       <c r="D11" s="9"/>
     </row>
-    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>23</v>
       </c>
@@ -1326,7 +1326,7 @@
       </c>
       <c r="D12" s="20"/>
     </row>
-    <row r="13" spans="1:4" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>24</v>
       </c>
@@ -1338,7 +1338,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
         <v>27</v>
       </c>
@@ -1348,7 +1348,7 @@
       </c>
       <c r="D14" s="24"/>
     </row>
-    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="21" t="s">
         <v>29</v>
       </c>
@@ -1358,7 +1358,7 @@
       </c>
       <c r="D15" s="24"/>
     </row>
-    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="21" t="s">
         <v>30</v>
       </c>
@@ -1366,7 +1366,7 @@
       <c r="C16" s="23"/>
       <c r="D16" s="25"/>
     </row>
-    <row r="17" spans="1:4" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="26" t="s">
         <v>31</v>
       </c>
@@ -1378,7 +1378,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="48.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="21" t="s">
         <v>34</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>36</v>
       </c>
@@ -1402,7 +1402,7 @@
       </c>
       <c r="D19" s="12"/>
     </row>
-    <row r="20" spans="1:4" ht="48.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="21" t="s">
         <v>38</v>
       </c>
@@ -1414,7 +1414,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>39</v>
       </c>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="D21" s="12"/>
     </row>
-    <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>41</v>
       </c>
@@ -1438,7 +1438,7 @@
       </c>
       <c r="D22" s="12"/>
     </row>
-    <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>42</v>
       </c>
@@ -1450,7 +1450,7 @@
       </c>
       <c r="D23" s="12"/>
     </row>
-    <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>44</v>
       </c>
@@ -1462,7 +1462,7 @@
       </c>
       <c r="D24" s="12"/>
     </row>
-    <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="21" t="s">
         <v>45</v>
       </c>
@@ -1472,7 +1472,7 @@
       </c>
       <c r="D25" s="25"/>
     </row>
-    <row r="26" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="21" t="s">
         <v>47</v>
       </c>
@@ -1482,7 +1482,7 @@
       </c>
       <c r="D26" s="25"/>
     </row>
-    <row r="27" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="21" t="s">
         <v>48</v>
       </c>
@@ -1492,7 +1492,7 @@
       </c>
       <c r="D27" s="24"/>
     </row>
-    <row r="28" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="21" t="s">
         <v>49</v>
       </c>
@@ -1502,7 +1502,7 @@
       </c>
       <c r="D28" s="24"/>
     </row>
-    <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>50</v>
       </c>
@@ -1512,7 +1512,7 @@
       </c>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" spans="1:4" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="26" t="s">
         <v>52</v>
       </c>
@@ -1524,7 +1524,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="21" t="s">
         <v>53</v>
       </c>
@@ -1534,7 +1534,7 @@
       </c>
       <c r="D31" s="29"/>
     </row>
-    <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="30" t="s">
         <v>54</v>
       </c>
@@ -1546,7 +1546,7 @@
       </c>
       <c r="D32" s="32"/>
     </row>
-    <row r="33" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="21" t="s">
         <v>55</v>
       </c>
@@ -1556,7 +1556,7 @@
       </c>
       <c r="D33" s="29"/>
     </row>
-    <row r="34" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="21" t="s">
         <v>56</v>
       </c>
@@ -1566,7 +1566,7 @@
       </c>
       <c r="D34" s="24"/>
     </row>
-    <row r="35" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="30" t="s">
         <v>57</v>
       </c>
@@ -1578,7 +1578,7 @@
       </c>
       <c r="D35" s="32"/>
     </row>
-    <row r="36" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="30" t="s">
         <v>58</v>
       </c>
@@ -1590,7 +1590,7 @@
       </c>
       <c r="D36" s="32"/>
     </row>
-    <row r="37" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="30" t="s">
         <v>59</v>
       </c>
@@ -1602,7 +1602,7 @@
       </c>
       <c r="D37" s="32"/>
     </row>
-    <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="30" t="s">
         <v>60</v>
       </c>
@@ -1614,7 +1614,7 @@
       </c>
       <c r="D38" s="32"/>
     </row>
-    <row r="39" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="21" t="s">
         <v>61</v>
       </c>
@@ -1624,7 +1624,7 @@
       </c>
       <c r="D39" s="24"/>
     </row>
-    <row r="40" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="17" t="s">
         <v>62</v>
       </c>
@@ -1634,7 +1634,7 @@
       </c>
       <c r="D40" s="20"/>
     </row>
-    <row r="41" spans="1:4" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="17" t="s">
         <v>64</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="48.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="33" t="s">
         <v>66</v>
       </c>
@@ -1658,7 +1658,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="21" t="s">
         <v>67</v>
       </c>
@@ -1668,7 +1668,7 @@
       </c>
       <c r="D43" s="24"/>
     </row>
-    <row r="44" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="30" t="s">
         <v>68</v>
       </c>
@@ -1680,7 +1680,7 @@
       </c>
       <c r="D44" s="32"/>
     </row>
-    <row r="45" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="21" t="s">
         <v>70</v>
       </c>
@@ -1690,7 +1690,7 @@
       </c>
       <c r="D45" s="25"/>
     </row>
-    <row r="46" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="21" t="s">
         <v>71</v>
       </c>
@@ -1698,7 +1698,7 @@
       <c r="C46" s="22"/>
       <c r="D46" s="29"/>
     </row>
-    <row r="47" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="21" t="s">
         <v>72</v>
       </c>
@@ -1706,7 +1706,7 @@
       <c r="C47" s="22"/>
       <c r="D47" s="25"/>
     </row>
-    <row r="48" spans="1:4" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="17" t="s">
         <v>73</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="21" t="s">
         <v>75</v>
       </c>
@@ -1726,7 +1726,7 @@
       </c>
       <c r="D49" s="24"/>
     </row>
-    <row r="50" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="14" t="s">
         <v>76</v>
       </c>
@@ -1736,7 +1736,7 @@
       </c>
       <c r="D50" s="16"/>
     </row>
-    <row r="51" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
         <v>78</v>
       </c>
@@ -1746,7 +1746,7 @@
       </c>
       <c r="D51" s="6"/>
     </row>
-    <row r="52" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="14" t="s">
         <v>80</v>
       </c>
@@ -1756,7 +1756,7 @@
       </c>
       <c r="D52" s="16"/>
     </row>
-    <row r="53" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="14" t="s">
         <v>82</v>
       </c>
@@ -1766,7 +1766,7 @@
       </c>
       <c r="D53" s="16"/>
     </row>
-    <row r="54" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="21" t="s">
         <v>84</v>
       </c>
@@ -1786,18 +1786,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{635BC677-F96E-418F-8F39-12F67BF3BECC}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>87</v>
       </c>
@@ -1814,7 +1814,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>88</v>
       </c>
@@ -1825,7 +1825,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>90</v>
       </c>
@@ -1836,7 +1836,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>91</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>93</v>
       </c>
@@ -1858,7 +1858,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>96</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>100</v>
       </c>
@@ -1880,7 +1880,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>105</v>
       </c>
@@ -1891,7 +1891,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>107</v>
       </c>
@@ -1902,7 +1902,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>109</v>
       </c>
@@ -1913,7 +1913,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>110</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>111</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>113</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>115</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>116</v>
       </c>
@@ -1968,7 +1968,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>118</v>
       </c>
@@ -1979,7 +1979,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>120</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>127</v>
       </c>
@@ -2001,7 +2001,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>128</v>
       </c>
@@ -2012,7 +2012,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>130</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>133</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>137</v>
       </c>
@@ -2045,7 +2045,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>98</v>
       </c>
@@ -2056,7 +2056,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>99</v>
       </c>
@@ -2067,7 +2067,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>119</v>
       </c>
@@ -2078,7 +2078,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>122</v>
       </c>
@@ -2089,7 +2089,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>123</v>
       </c>
@@ -2100,7 +2100,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>125</v>
       </c>
@@ -2111,7 +2111,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>126</v>
       </c>
@@ -2122,7 +2122,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>135</v>
       </c>
@@ -2133,7 +2133,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -2144,7 +2144,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>95</v>
       </c>
@@ -2158,7 +2158,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>102</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>103</v>
       </c>
@@ -2180,7 +2180,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -2191,7 +2191,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>104</v>
       </c>
@@ -2205,7 +2205,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>124</v>
       </c>
@@ -2216,7 +2216,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>132</v>
       </c>
@@ -2227,7 +2227,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -2238,7 +2238,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>136</v>
       </c>
@@ -2263,7 +2263,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>139</v>
       </c>
@@ -2274,7 +2274,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>89</v>
       </c>
@@ -2285,7 +2285,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>92</v>
       </c>
@@ -2296,7 +2296,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>94</v>
       </c>
@@ -2307,7 +2307,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>97</v>
       </c>
@@ -2318,7 +2318,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>101</v>
       </c>
@@ -2329,7 +2329,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>106</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>108</v>
       </c>
@@ -2351,7 +2351,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>112</v>
       </c>
@@ -2362,7 +2362,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>114</v>
       </c>
@@ -2373,7 +2373,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>117</v>
       </c>
@@ -2384,7 +2384,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>121</v>
       </c>
@@ -2395,7 +2395,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>129</v>
       </c>
@@ -2406,7 +2406,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>131</v>
       </c>
@@ -2417,7 +2417,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>134</v>
       </c>
@@ -2428,7 +2428,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>138</v>
       </c>

</xml_diff>

<commit_message>
formatting and adjusting column names
</commit_message>
<xml_diff>
--- a/extdata/biochem_dictionary.xlsx
+++ b/extdata/biochem_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ogradye\Documents\Davis_Strait\R_Working\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BED7CEB-B6CF-4C97-9EEF-4F99B9855657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5EDA52F-2AED-4484-AB03-2E8A9B708EB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BCS" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="191">
   <si>
     <t>Header</t>
   </si>
@@ -481,12 +481,6 @@
     <t>COLLECTOR_EVENT_ID</t>
   </si>
   <si>
-    <t>HEADER_START_LAT</t>
-  </si>
-  <si>
-    <t>HEADER_START_LON</t>
-  </si>
-  <si>
     <t>NO2NO3_0</t>
   </si>
   <si>
@@ -532,9 +526,6 @@
     <t>O18_Water</t>
   </si>
   <si>
-    <t>EVENT_START</t>
-  </si>
-  <si>
     <t>qc</t>
   </si>
   <si>
@@ -550,15 +541,9 @@
     <t>SOUNDING</t>
   </si>
   <si>
-    <t>START_TIME</t>
-  </si>
-  <si>
     <t>GO-SHIP</t>
   </si>
   <si>
-    <t>START_DATE</t>
-  </si>
-  <si>
     <t>NH3_0_qc</t>
   </si>
   <si>
@@ -602,6 +587,18 @@
   </si>
   <si>
     <t>O18_Water_qc</t>
+  </si>
+  <si>
+    <t>DIS_HEADER_SDATE</t>
+  </si>
+  <si>
+    <t>DIS_HEADER_SLAT</t>
+  </si>
+  <si>
+    <t>DIS_HEADER_SLON</t>
+  </si>
+  <si>
+    <t>DIS_HEADER_STIME</t>
   </si>
 </sst>
 </file>
@@ -1187,19 +1184,19 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.5703125" customWidth="1"/>
-    <col min="3" max="3" width="56.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5546875" customWidth="1"/>
+    <col min="3" max="3" width="56.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -1208,7 +1205,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1218,7 +1215,7 @@
       </c>
       <c r="D2" s="6"/>
     </row>
-    <row r="3" spans="1:4" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
@@ -1227,10 +1224,10 @@
         <v>6</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>7</v>
       </c>
@@ -1242,7 +1239,7 @@
       </c>
       <c r="D4" s="12"/>
     </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
         <v>9</v>
       </c>
@@ -1254,7 +1251,7 @@
       </c>
       <c r="D5" s="13"/>
     </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
         <v>11</v>
       </c>
@@ -1266,7 +1263,7 @@
       </c>
       <c r="D6" s="13"/>
     </row>
-    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>13</v>
       </c>
@@ -1276,7 +1273,7 @@
       </c>
       <c r="D7" s="9"/>
     </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>15</v>
       </c>
@@ -1286,7 +1283,7 @@
       </c>
       <c r="D8" s="9"/>
     </row>
-    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>17</v>
       </c>
@@ -1296,7 +1293,7 @@
       </c>
       <c r="D9" s="9"/>
     </row>
-    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
         <v>19</v>
       </c>
@@ -1306,7 +1303,7 @@
       </c>
       <c r="D10" s="16"/>
     </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>21</v>
       </c>
@@ -1316,17 +1313,17 @@
       </c>
       <c r="D11" s="9"/>
     </row>
-    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="17" t="s">
         <v>23</v>
       </c>
       <c r="B12" s="19"/>
       <c r="C12" s="19" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D12" s="20"/>
     </row>
-    <row r="13" spans="1:4" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>24</v>
       </c>
@@ -1338,7 +1335,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="21" t="s">
         <v>27</v>
       </c>
@@ -1348,7 +1345,7 @@
       </c>
       <c r="D14" s="24"/>
     </row>
-    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="21" t="s">
         <v>29</v>
       </c>
@@ -1358,7 +1355,7 @@
       </c>
       <c r="D15" s="24"/>
     </row>
-    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="21" t="s">
         <v>30</v>
       </c>
@@ -1366,7 +1363,7 @@
       <c r="C16" s="23"/>
       <c r="D16" s="25"/>
     </row>
-    <row r="17" spans="1:4" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="26" t="s">
         <v>31</v>
       </c>
@@ -1378,7 +1375,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="48.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="21" t="s">
         <v>34</v>
       </c>
@@ -1390,7 +1387,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="s">
         <v>36</v>
       </c>
@@ -1402,7 +1399,7 @@
       </c>
       <c r="D19" s="12"/>
     </row>
-    <row r="20" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="48.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="21" t="s">
         <v>38</v>
       </c>
@@ -1414,7 +1411,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
         <v>39</v>
       </c>
@@ -1426,7 +1423,7 @@
       </c>
       <c r="D21" s="12"/>
     </row>
-    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="10" t="s">
         <v>41</v>
       </c>
@@ -1438,7 +1435,7 @@
       </c>
       <c r="D22" s="12"/>
     </row>
-    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="10" t="s">
         <v>42</v>
       </c>
@@ -1450,7 +1447,7 @@
       </c>
       <c r="D23" s="12"/>
     </row>
-    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="10" t="s">
         <v>44</v>
       </c>
@@ -1462,7 +1459,7 @@
       </c>
       <c r="D24" s="12"/>
     </row>
-    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="21" t="s">
         <v>45</v>
       </c>
@@ -1472,7 +1469,7 @@
       </c>
       <c r="D25" s="25"/>
     </row>
-    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="21" t="s">
         <v>47</v>
       </c>
@@ -1482,7 +1479,7 @@
       </c>
       <c r="D26" s="25"/>
     </row>
-    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="21" t="s">
         <v>48</v>
       </c>
@@ -1492,7 +1489,7 @@
       </c>
       <c r="D27" s="24"/>
     </row>
-    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="21" t="s">
         <v>49</v>
       </c>
@@ -1502,7 +1499,7 @@
       </c>
       <c r="D28" s="24"/>
     </row>
-    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>50</v>
       </c>
@@ -1512,7 +1509,7 @@
       </c>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" spans="1:4" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="26" t="s">
         <v>52</v>
       </c>
@@ -1524,7 +1521,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="21" t="s">
         <v>53</v>
       </c>
@@ -1534,7 +1531,7 @@
       </c>
       <c r="D31" s="29"/>
     </row>
-    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="30" t="s">
         <v>54</v>
       </c>
@@ -1546,7 +1543,7 @@
       </c>
       <c r="D32" s="32"/>
     </row>
-    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="21" t="s">
         <v>55</v>
       </c>
@@ -1556,7 +1553,7 @@
       </c>
       <c r="D33" s="29"/>
     </row>
-    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="21" t="s">
         <v>56</v>
       </c>
@@ -1566,7 +1563,7 @@
       </c>
       <c r="D34" s="24"/>
     </row>
-    <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="30" t="s">
         <v>57</v>
       </c>
@@ -1578,7 +1575,7 @@
       </c>
       <c r="D35" s="32"/>
     </row>
-    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="30" t="s">
         <v>58</v>
       </c>
@@ -1590,7 +1587,7 @@
       </c>
       <c r="D36" s="32"/>
     </row>
-    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="30" t="s">
         <v>59</v>
       </c>
@@ -1602,7 +1599,7 @@
       </c>
       <c r="D37" s="32"/>
     </row>
-    <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="30" t="s">
         <v>60</v>
       </c>
@@ -1614,7 +1611,7 @@
       </c>
       <c r="D38" s="32"/>
     </row>
-    <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="21" t="s">
         <v>61</v>
       </c>
@@ -1624,7 +1621,7 @@
       </c>
       <c r="D39" s="24"/>
     </row>
-    <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="17" t="s">
         <v>62</v>
       </c>
@@ -1634,7 +1631,7 @@
       </c>
       <c r="D40" s="20"/>
     </row>
-    <row r="41" spans="1:4" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="17" t="s">
         <v>64</v>
       </c>
@@ -1644,7 +1641,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="48.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="33" t="s">
         <v>66</v>
       </c>
@@ -1658,7 +1655,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="21" t="s">
         <v>67</v>
       </c>
@@ -1668,7 +1665,7 @@
       </c>
       <c r="D43" s="24"/>
     </row>
-    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="30" t="s">
         <v>68</v>
       </c>
@@ -1680,7 +1677,7 @@
       </c>
       <c r="D44" s="32"/>
     </row>
-    <row r="45" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="21" t="s">
         <v>70</v>
       </c>
@@ -1690,7 +1687,7 @@
       </c>
       <c r="D45" s="25"/>
     </row>
-    <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="21" t="s">
         <v>71</v>
       </c>
@@ -1698,7 +1695,7 @@
       <c r="C46" s="22"/>
       <c r="D46" s="29"/>
     </row>
-    <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="21" t="s">
         <v>72</v>
       </c>
@@ -1706,7 +1703,7 @@
       <c r="C47" s="22"/>
       <c r="D47" s="25"/>
     </row>
-    <row r="48" spans="1:4" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="17" t="s">
         <v>73</v>
       </c>
@@ -1716,7 +1713,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="21" t="s">
         <v>75</v>
       </c>
@@ -1726,7 +1723,7 @@
       </c>
       <c r="D49" s="24"/>
     </row>
-    <row r="50" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="14" t="s">
         <v>76</v>
       </c>
@@ -1736,7 +1733,7 @@
       </c>
       <c r="D50" s="16"/>
     </row>
-    <row r="51" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
         <v>78</v>
       </c>
@@ -1746,7 +1743,7 @@
       </c>
       <c r="D51" s="6"/>
     </row>
-    <row r="52" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="14" t="s">
         <v>80</v>
       </c>
@@ -1756,7 +1753,7 @@
       </c>
       <c r="D52" s="16"/>
     </row>
-    <row r="53" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="14" t="s">
         <v>82</v>
       </c>
@@ -1766,7 +1763,7 @@
       </c>
       <c r="D53" s="16"/>
     </row>
-    <row r="54" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="21" t="s">
         <v>84</v>
       </c>
@@ -1786,18 +1783,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{635BC677-F96E-418F-8F39-12F67BF3BECC}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>87</v>
       </c>
@@ -1814,18 +1811,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>88</v>
       </c>
       <c r="B2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>90</v>
       </c>
@@ -1836,7 +1833,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>91</v>
       </c>
@@ -1847,7 +1844,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>93</v>
       </c>
@@ -1858,7 +1855,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>96</v>
       </c>
@@ -1869,7 +1866,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>100</v>
       </c>
@@ -1880,117 +1877,117 @@
         <v>143</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>105</v>
       </c>
       <c r="B8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D8" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>107</v>
       </c>
       <c r="B9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D9" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>109</v>
       </c>
       <c r="B10" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D10" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>110</v>
       </c>
       <c r="B11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D11" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>111</v>
       </c>
       <c r="B12" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D12" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>113</v>
       </c>
       <c r="B13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D13" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>115</v>
       </c>
       <c r="B14" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D14" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>116</v>
       </c>
       <c r="B15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D15" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>118</v>
       </c>
       <c r="B16" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D16" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>120</v>
       </c>
       <c r="B17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D17" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>127</v>
       </c>
@@ -2001,7 +1998,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>128</v>
       </c>
@@ -2012,40 +2009,40 @@
         <v>143</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>130</v>
       </c>
       <c r="B20" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D20" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>133</v>
       </c>
       <c r="B21" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D21" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>137</v>
       </c>
       <c r="B22" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D22" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>98</v>
       </c>
@@ -2056,7 +2053,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>99</v>
       </c>
@@ -2067,73 +2064,73 @@
         <v>148</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>119</v>
       </c>
       <c r="B25" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D25" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>122</v>
       </c>
       <c r="B26" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D26" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>123</v>
       </c>
       <c r="B27" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D27" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>125</v>
       </c>
       <c r="B28" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D28" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>126</v>
       </c>
       <c r="B29" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D29" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>135</v>
       </c>
       <c r="B30" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D30" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -2144,7 +2141,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>95</v>
       </c>
@@ -2155,10 +2152,10 @@
         <v>145</v>
       </c>
       <c r="E32" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>102</v>
       </c>
@@ -2169,29 +2166,29 @@
         <v>145</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>103</v>
       </c>
       <c r="B34" t="s">
-        <v>151</v>
+        <v>188</v>
       </c>
       <c r="D34" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>43</v>
       </c>
       <c r="B35" t="s">
-        <v>152</v>
+        <v>189</v>
       </c>
       <c r="D35" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>104</v>
       </c>
@@ -2202,54 +2199,54 @@
         <v>145</v>
       </c>
       <c r="E36" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>124</v>
       </c>
       <c r="B37" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D37" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>132</v>
       </c>
       <c r="B38" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D38" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D39" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>37</v>
       </c>
       <c r="B40" t="s">
-        <v>174</v>
+        <v>190</v>
       </c>
       <c r="D40" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>136</v>
       </c>
@@ -2260,183 +2257,183 @@
         <v>145</v>
       </c>
       <c r="E41" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>139</v>
       </c>
       <c r="B42" t="s">
-        <v>168</v>
+        <v>187</v>
       </c>
       <c r="D42" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>89</v>
       </c>
       <c r="B43" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="D43" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>92</v>
       </c>
       <c r="B44" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="D44" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>94</v>
       </c>
       <c r="B45" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D45" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>97</v>
       </c>
       <c r="B46" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="D46" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>101</v>
       </c>
       <c r="B47" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="D47" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>106</v>
       </c>
       <c r="B48" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D48" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>108</v>
       </c>
       <c r="B49" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D49" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>112</v>
       </c>
       <c r="B50" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D50" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>114</v>
       </c>
       <c r="B51" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D51" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>117</v>
       </c>
       <c r="B52" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="D52" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>121</v>
       </c>
       <c r="B53" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D53" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>129</v>
       </c>
       <c r="B54" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="D54" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>131</v>
       </c>
       <c r="B55" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="D55" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>134</v>
       </c>
       <c r="B56" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D56" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>138</v>
       </c>
       <c r="B57" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D57" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>